<commit_message>
For Beyesian histogram creation, centered the bins around the min and max values to get better accuracy.
</commit_message>
<xml_diff>
--- a/assignments/assignment2/Assignment_2_Data_and_Template - Output.xlsx
+++ b/assignments/assignment2/Assignment_2_Data_and_Template - Output.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\git\Machine-Learning\UCSC-Extension\assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\git\Machine-Learning\UCSC-Extension\assignments\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -532,6 +532,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,9 +549,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3012,7 +3012,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B14"/>
+      <selection activeCell="B7" sqref="B7:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4420,7 +4420,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5841,7 +5841,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -5855,7 +5855,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
@@ -5871,10 +5871,10 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="10">
@@ -5886,8 +5886,8 @@
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="12">
         <v>1.65170135</v>
       </c>
@@ -5897,8 +5897,8 @@
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="10">
@@ -5910,8 +5910,8 @@
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="12">
         <v>1.8015734299999999</v>
       </c>
@@ -5925,7 +5925,7 @@
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -5936,7 +5936,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="25" t="s">
         <v>4</v>
       </c>
@@ -5976,14 +5976,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="7" t="s">
         <v>26</v>
       </c>
@@ -6072,8 +6072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6253,32 +6253,32 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="32" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="17">
-        <v>0.26082460454536233</v>
+        <v>0.42181000741967262</v>
       </c>
       <c r="C7" s="17">
-        <v>0.85277087417737829</v>
+        <v>1.416127611022489</v>
       </c>
       <c r="D7" s="17">
-        <v>0.91837650200974708</v>
+        <v>1.114682176238323</v>
       </c>
       <c r="E7" s="17">
-        <v>0.32577201217394419</v>
+        <v>0.2057135400897718</v>
       </c>
       <c r="F7" s="17">
-        <v>3.8063733187597537E-2</v>
+        <v>8.900980589087398E-3</v>
       </c>
       <c r="G7" s="17">
-        <v>1.4649189382565739E-3</v>
+        <v>9.0297553707593129E-5</v>
       </c>
       <c r="H7" s="17">
-        <v>1.8570363703477861E-5</v>
+        <v>2.1477180670160721E-7</v>
       </c>
       <c r="I7" s="17">
-        <v>7.754107694549267E-8</v>
+        <v>1.197682519903858E-10</v>
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -6306,30 +6306,30 @@
       <c r="AG7" s="17"/>
     </row>
     <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="17">
-        <v>0.57530796515041249</v>
+        <v>0.91903144854048935</v>
       </c>
       <c r="C8" s="17">
-        <v>3.0166455107940719</v>
+        <v>5.7181291714131923</v>
       </c>
       <c r="D8" s="20">
-        <v>5.2101805535428891</v>
+        <v>8.3414337627574753</v>
       </c>
       <c r="E8" s="20">
-        <v>2.964052361204184</v>
+        <v>2.8529266384953669</v>
       </c>
       <c r="F8" s="20">
-        <v>0.55542263193898533</v>
+        <v>0.22877241545696711</v>
       </c>
       <c r="G8" s="20">
-        <v>3.4281978303945519E-2</v>
+        <v>4.3011032288181464E-3</v>
       </c>
       <c r="H8" s="20">
-        <v>6.9696790947971468E-4</v>
+        <v>1.8959166003158948E-5</v>
       </c>
       <c r="I8" s="17">
-        <v>4.6672846850080574E-6</v>
+        <v>1.9593938801572318E-8</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -6358,28 +6358,28 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" s="17">
-        <v>0.46513285239665358</v>
+        <v>0.53980571875664418</v>
       </c>
       <c r="C9" s="18">
-        <v>3.9114789495356632</v>
-      </c>
-      <c r="D9" s="20">
-        <v>10.834517683469359</v>
-      </c>
-      <c r="E9" s="20">
-        <v>9.8851387852670651</v>
-      </c>
-      <c r="F9" s="20">
-        <v>2.9707120810729428</v>
-      </c>
-      <c r="G9" s="20">
-        <v>0.29406474224499102</v>
-      </c>
-      <c r="H9" s="20">
-        <v>9.588042574373545E-3</v>
+        <v>6.2244236991578212</v>
+      </c>
+      <c r="D9" s="17">
+        <v>16.82766930954692</v>
+      </c>
+      <c r="E9" s="17">
+        <v>10.66625457620702</v>
+      </c>
+      <c r="F9" s="17">
+        <v>1.5851233954784689</v>
+      </c>
+      <c r="G9" s="17">
+        <v>5.5230294856854253E-2</v>
+      </c>
+      <c r="H9" s="17">
+        <v>4.5118515556225828E-4</v>
       </c>
       <c r="I9" s="19">
-        <v>1.0297257044130241E-4</v>
+        <v>8.6416246361907205E-7</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -6408,28 +6408,28 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
-        <v>0.13784100838467431</v>
+        <v>8.5474821826217379E-2</v>
       </c>
       <c r="C10" s="18">
-        <v>1.859013375920467</v>
-      </c>
-      <c r="D10" s="20">
-        <v>8.258310175438881</v>
-      </c>
-      <c r="E10" s="20">
-        <v>12.083826179796191</v>
-      </c>
-      <c r="F10" s="20">
-        <v>5.8240132102931472</v>
-      </c>
-      <c r="G10" s="20">
-        <v>0.92458072685127413</v>
-      </c>
-      <c r="H10" s="20">
-        <v>4.834726642928814E-2</v>
+        <v>1.826576845595417</v>
+      </c>
+      <c r="D10" s="17">
+        <v>9.1516804371411737</v>
+      </c>
+      <c r="E10" s="17">
+        <v>10.75045635616919</v>
+      </c>
+      <c r="F10" s="17">
+        <v>2.9608479737258659</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0.1911914523373156</v>
+      </c>
+      <c r="H10" s="17">
+        <v>2.8945695584442969E-3</v>
       </c>
       <c r="I10" s="19">
-        <v>8.3272885679373245E-4</v>
+        <v>1.027454653499464E-5</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -6458,28 +6458,28 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
-        <v>1.4972856659342349E-2</v>
+        <v>3.648652826983699E-3</v>
       </c>
       <c r="C11" s="18">
-        <v>0.32385367567261208</v>
-      </c>
-      <c r="D11" s="20">
-        <v>2.3072656323841652</v>
-      </c>
-      <c r="E11" s="20">
-        <v>5.4144078496003134</v>
-      </c>
-      <c r="F11" s="20">
-        <v>4.1851298684407636</v>
-      </c>
-      <c r="G11" s="20">
-        <v>1.065544310479579</v>
-      </c>
-      <c r="H11" s="20">
-        <v>8.9359080820279727E-2</v>
+        <v>0.14450083715292281</v>
+      </c>
+      <c r="D11" s="17">
+        <v>1.3417491826025061</v>
+      </c>
+      <c r="E11" s="17">
+        <v>2.921026321825543</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1.4909488914966049</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.1784239695563479</v>
+      </c>
+      <c r="H11" s="17">
+        <v>5.0061838282779141E-3</v>
       </c>
       <c r="I11" s="19">
-        <v>2.468371219910268E-3</v>
+        <v>3.2932412266226138E-5</v>
       </c>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -6508,28 +6508,28 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" s="17">
-        <v>5.9615019593203941E-4</v>
+        <v>4.1987546129869399E-5</v>
       </c>
       <c r="C12" s="18">
-        <v>2.0679495775848541E-2</v>
-      </c>
-      <c r="D12" s="20">
-        <v>0.23628100116847231</v>
-      </c>
-      <c r="E12" s="20">
-        <v>0.8892467005669481</v>
-      </c>
-      <c r="F12" s="20">
-        <v>1.1023520789918231</v>
-      </c>
-      <c r="G12" s="20">
-        <v>0.45011448749238481</v>
-      </c>
-      <c r="H12" s="20">
-        <v>6.0538305462274691E-2</v>
+        <v>3.081742820322462E-3</v>
+      </c>
+      <c r="D12" s="17">
+        <v>5.3031687468430101E-2</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.2139624958160839</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.2023965095857363</v>
+      </c>
+      <c r="G12" s="17">
+        <v>4.488813242929774E-2</v>
+      </c>
+      <c r="H12" s="17">
+        <v>2.3341201625000831E-3</v>
       </c>
       <c r="I12" s="19">
-        <v>2.681897233194017E-3</v>
+        <v>2.8456274277932191E-5</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -6558,28 +6558,28 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" s="17">
-        <v>8.7002456255774249E-6</v>
+        <v>1.3025729671541579E-7</v>
       </c>
       <c r="C13" s="18">
-        <v>4.8401169847627509E-4</v>
-      </c>
-      <c r="D13" s="20">
-        <v>8.8692073109506598E-3</v>
-      </c>
-      <c r="E13" s="20">
-        <v>5.3532602470688077E-2</v>
-      </c>
-      <c r="F13" s="20">
-        <v>0.1064281494009417</v>
-      </c>
-      <c r="G13" s="20">
-        <v>6.9694622029008169E-2</v>
-      </c>
-      <c r="H13" s="20">
-        <v>1.503303354790581E-2</v>
+        <v>1.7718054662105831E-5</v>
+      </c>
+      <c r="D13" s="17">
+        <v>5.6505818273271786E-4</v>
+      </c>
+      <c r="E13" s="17">
+        <v>4.2250655819288992E-3</v>
+      </c>
+      <c r="F13" s="17">
+        <v>7.4069070631309084E-3</v>
+      </c>
+      <c r="G13" s="17">
+        <v>3.044412463732844E-3</v>
+      </c>
+      <c r="H13" s="17">
+        <v>2.9338184940709718E-4</v>
       </c>
       <c r="I13" s="19">
-        <v>1.06806722667593E-3</v>
+        <v>6.6286661646403436E-6</v>
       </c>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
@@ -6608,28 +6608,28 @@
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17">
-        <v>4.6540616865814417E-8</v>
+        <v>1.089374593268692E-10</v>
       </c>
       <c r="C14" s="18">
-        <v>4.1523750287238556E-6</v>
-      </c>
-      <c r="D14" s="20">
-        <v>1.220297183647122E-4</v>
-      </c>
-      <c r="E14" s="20">
-        <v>1.181243006227839E-3</v>
-      </c>
-      <c r="F14" s="20">
-        <v>3.7663224103154E-3</v>
-      </c>
-      <c r="G14" s="20">
-        <v>3.9554904610977493E-3</v>
-      </c>
-      <c r="H14" s="20">
-        <v>1.3683203678064621E-3</v>
+        <v>2.746181873183145E-8</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1.623097111509683E-6</v>
+      </c>
+      <c r="E14" s="17">
+        <v>2.24917303641729E-5</v>
+      </c>
+      <c r="F14" s="17">
+        <v>7.3074253404499707E-5</v>
+      </c>
+      <c r="G14" s="17">
+        <v>5.5663314133558052E-5</v>
+      </c>
+      <c r="H14" s="17">
+        <v>9.9411559864538276E-6</v>
       </c>
       <c r="I14" s="19">
-        <v>1.559121084220316E-4</v>
+        <v>4.1626305897347482E-7</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
@@ -7485,7 +7485,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7665,32 +7665,32 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="32" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="17">
-        <v>1.303280946778704E-5</v>
+        <v>2.5298683390901781E-5</v>
       </c>
       <c r="C7" s="17">
-        <v>3.1268802829124357E-4</v>
+        <v>8.1137725825714186E-4</v>
       </c>
       <c r="D7" s="17">
-        <v>2.149500903269382E-3</v>
+        <v>5.0853788328569759E-3</v>
       </c>
       <c r="E7" s="17">
-        <v>4.2336717240967769E-3</v>
+        <v>6.2287279156408148E-3</v>
       </c>
       <c r="F7" s="17">
-        <v>2.389185654472048E-3</v>
+        <v>1.490908459300956E-3</v>
       </c>
       <c r="G7" s="17">
-        <v>3.8630985456499428E-4</v>
+        <v>6.973939358140292E-5</v>
       </c>
       <c r="H7" s="17">
-        <v>1.789677777910857E-5</v>
+        <v>6.3750107816174563E-7</v>
       </c>
       <c r="I7" s="17">
-        <v>2.3755658553052031E-7</v>
+        <v>1.138830919312522E-9</v>
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -7718,30 +7718,30 @@
       <c r="AG7" s="17"/>
     </row>
     <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="17">
-        <v>5.0031884334658551E-5</v>
+        <v>1.061464886145967E-4</v>
       </c>
       <c r="C8" s="17">
-        <v>1.9679722805901732E-3</v>
-      </c>
-      <c r="D8" s="17">
-        <v>2.217911762974353E-2</v>
-      </c>
-      <c r="E8" s="17">
-        <v>7.1618087885233619E-2</v>
-      </c>
-      <c r="F8" s="17">
-        <v>6.6260445163856735E-2</v>
-      </c>
-      <c r="G8" s="17">
-        <v>1.7564635715513841E-2</v>
-      </c>
-      <c r="H8" s="17">
-        <v>1.3340653831157611E-3</v>
+        <v>6.4931226759654048E-3</v>
+      </c>
+      <c r="D8" s="20">
+        <v>7.7620628245214665E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0.1813327584170846</v>
+      </c>
+      <c r="F8" s="20">
+        <v>8.2784866313152142E-2</v>
+      </c>
+      <c r="G8" s="20">
+        <v>7.3858622696637488E-3</v>
+      </c>
+      <c r="H8" s="20">
+        <v>1.2877365629887819E-4</v>
       </c>
       <c r="I8" s="17">
-        <v>2.9031418288618098E-5</v>
+        <v>4.387614047295237E-7</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -7770,28 +7770,28 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" s="17">
-        <v>7.9678611883246089E-5</v>
-      </c>
-      <c r="C9" s="17">
-        <v>5.138221071811673E-3</v>
-      </c>
-      <c r="D9" s="17">
-        <v>9.4937323195254983E-2</v>
-      </c>
-      <c r="E9" s="17">
-        <v>0.5025905854935474</v>
-      </c>
-      <c r="F9" s="17">
-        <v>0.76233329150150153</v>
-      </c>
-      <c r="G9" s="17">
-        <v>0.33130545993122468</v>
-      </c>
-      <c r="H9" s="17">
-        <v>4.1253943588759362E-2</v>
-      </c>
-      <c r="I9" s="17">
-        <v>1.471822771245111E-3</v>
+        <v>1.4113209318419059E-4</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1.646633035231165E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.37544250133670432</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1.6728831792896679</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1.4566773363662</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.24787725692085011</v>
+      </c>
+      <c r="H9" s="18">
+        <v>8.2430051054350542E-3</v>
+      </c>
+      <c r="I9" s="19">
+        <v>5.3568566576318982E-5</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -7820,28 +7820,28 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
-        <v>5.2640832007885402E-5</v>
-      </c>
-      <c r="C10" s="17">
-        <v>5.5653525450862773E-3</v>
-      </c>
-      <c r="D10" s="17">
-        <v>0.16858377961236889</v>
-      </c>
-      <c r="E10" s="17">
-        <v>1.4631608172780171</v>
-      </c>
-      <c r="F10" s="17">
-        <v>3.6384927059911401</v>
-      </c>
-      <c r="G10" s="17">
-        <v>2.5924126084104442</v>
-      </c>
-      <c r="H10" s="17">
-        <v>0.52922446378777033</v>
-      </c>
-      <c r="I10" s="17">
-        <v>3.0954861718726811E-2</v>
+        <v>5.9464582240038733E-5</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1.32328222445367E-2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.57546929269824276</v>
+      </c>
+      <c r="E10" s="18">
+        <v>4.8906591866759603</v>
+      </c>
+      <c r="F10" s="18">
+        <v>8.1224718244910399</v>
+      </c>
+      <c r="G10" s="18">
+        <v>2.6362378846929122</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.16720780640891339</v>
+      </c>
+      <c r="I10" s="19">
+        <v>2.0725454880322872E-3</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -7870,28 +7870,28 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
-        <v>1.44274579133129E-5</v>
-      </c>
-      <c r="C11" s="17">
-        <v>2.500683111463052E-3</v>
-      </c>
-      <c r="D11" s="17">
-        <v>0.1241882983187538</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1.7670785760903771</v>
-      </c>
-      <c r="F11" s="17">
-        <v>7.2041743884830289</v>
-      </c>
-      <c r="G11" s="17">
-        <v>8.4152252019863987</v>
-      </c>
-      <c r="H11" s="17">
-        <v>2.816439577768298</v>
-      </c>
-      <c r="I11" s="17">
-        <v>0.27007743763408198</v>
+        <v>7.9396873341708461E-6</v>
+      </c>
+      <c r="C11" s="18">
+        <v>3.3699276109166679E-3</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.2795202736908986</v>
+      </c>
+      <c r="E11" s="18">
+        <v>4.5308702239605774</v>
+      </c>
+      <c r="F11" s="18">
+        <v>14.352432147277041</v>
+      </c>
+      <c r="G11" s="18">
+        <v>8.8847446569881043</v>
+      </c>
+      <c r="H11" s="18">
+        <v>1.0748304677045419</v>
+      </c>
+      <c r="I11" s="19">
+        <v>2.5410344652414971E-2</v>
       </c>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -7920,28 +7920,28 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" s="17">
-        <v>1.640374362970438E-6</v>
-      </c>
-      <c r="C12" s="17">
-        <v>4.6613394178474842E-4</v>
-      </c>
-      <c r="D12" s="17">
-        <v>3.7951736489022413E-2</v>
-      </c>
-      <c r="E12" s="17">
-        <v>0.8853311532245155</v>
-      </c>
-      <c r="F12" s="17">
-        <v>5.9174283944995949</v>
-      </c>
-      <c r="G12" s="17">
-        <v>11.3321795322097</v>
-      </c>
-      <c r="H12" s="17">
-        <v>6.2179475084194387</v>
-      </c>
-      <c r="I12" s="17">
-        <v>0.97753840051881746</v>
+        <v>3.3593934173342759E-7</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2.7195753983211588E-4</v>
+      </c>
+      <c r="D12" s="18">
+        <v>4.3024606795226891E-2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1.3301734811338839</v>
+      </c>
+      <c r="F12" s="18">
+        <v>8.0366532358302418</v>
+      </c>
+      <c r="G12" s="18">
+        <v>9.4889409413458594</v>
+      </c>
+      <c r="H12" s="18">
+        <v>2.1894540070152262</v>
+      </c>
+      <c r="I12" s="19">
+        <v>9.8725531100667743E-2</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -7970,28 +7970,28 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" s="17">
-        <v>7.7371713699175648E-8</v>
-      </c>
-      <c r="C13" s="17">
-        <v>3.6045319524517818E-5</v>
-      </c>
-      <c r="D13" s="17">
-        <v>4.8113695290940466E-3</v>
-      </c>
-      <c r="E13" s="17">
-        <v>0.18401012373056139</v>
-      </c>
-      <c r="F13" s="17">
-        <v>2.0163591550340558</v>
-      </c>
-      <c r="G13" s="17">
-        <v>6.3306344344788616</v>
-      </c>
-      <c r="H13" s="17">
-        <v>5.6948167026340117</v>
-      </c>
-      <c r="I13" s="17">
-        <v>1.4677951040280131</v>
+        <v>4.5043359281798892E-9</v>
+      </c>
+      <c r="C13" s="18">
+        <v>6.9549509966070194E-6</v>
+      </c>
+      <c r="D13" s="18">
+        <v>2.0986158361249842E-3</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.1237506207998026</v>
+      </c>
+      <c r="F13" s="18">
+        <v>1.426058678752441</v>
+      </c>
+      <c r="G13" s="18">
+        <v>3.2114633859800841</v>
+      </c>
+      <c r="H13" s="18">
+        <v>1.4133317753386221</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0.1215516449469676</v>
       </c>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
@@ -8020,28 +8020,28 @@
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17">
-        <v>1.5139360999268119E-9</v>
-      </c>
-      <c r="C14" s="17">
-        <v>1.1563069014794869E-6</v>
-      </c>
-      <c r="D14" s="17">
-        <v>2.5304156260016141E-4</v>
-      </c>
-      <c r="E14" s="17">
-        <v>1.586586570828815E-2</v>
-      </c>
-      <c r="F14" s="17">
-        <v>0.28502887416646111</v>
-      </c>
-      <c r="G14" s="17">
-        <v>1.467124977574487</v>
-      </c>
-      <c r="H14" s="17">
-        <v>2.16370742135567</v>
-      </c>
-      <c r="I14" s="17">
-        <v>0.91428822919588526</v>
+        <v>1.9138730025058501E-11</v>
+      </c>
+      <c r="C14" s="18">
+        <v>5.6363698559542399E-8</v>
+      </c>
+      <c r="D14" s="18">
+        <v>3.2438549033978197E-5</v>
+      </c>
+      <c r="E14" s="18">
+        <v>3.6483704195022291E-3</v>
+      </c>
+      <c r="F14" s="18">
+        <v>8.0188483594080207E-2</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0.34442974090914957</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0.28911116140189053</v>
+      </c>
+      <c r="I14" s="19">
+        <v>4.7424705306046443E-2</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
@@ -8896,7 +8896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8906,7 +8906,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="372" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>